<commit_message>
aanpassingen voor 3.0 nav consultatie
</commit_message>
<xml_diff>
--- a/11-relevante eigenschappen van het net/IMKL-Ordening-attributen-viewer-REVN-(2024-09-30).xlsx
+++ b/11-relevante eigenschappen van het net/IMKL-Ordening-attributen-viewer-REVN-(2024-09-30).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\p.janssen.GNM\Documents\Github\imkl-werkomgeving\11-relevante eigenschappen van het net\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7800FFCF-D953-449D-A70F-2830ABFEB557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0310EED4-5C5C-41E0-9CD3-ADB6AE214BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-8010" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="6" xr2:uid="{149DC1E7-FAE5-417C-8DC6-87A35A16D8AD}"/>
+    <workbookView xWindow="-28920" yWindow="-8010" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{149DC1E7-FAE5-417C-8DC6-87A35A16D8AD}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="9" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4966" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4968" uniqueCount="488">
   <si>
     <t>omschrijving</t>
   </si>
@@ -1604,6 +1604,9 @@
   </si>
   <si>
     <t>info per kabel</t>
+  </si>
+  <si>
+    <t>REVN 20240903 cardinaliteit van kablediameter 0..1</t>
   </si>
 </sst>
 </file>
@@ -2587,7 +2590,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="39" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="561">
+  <cellXfs count="562">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3600,7 +3603,10 @@
     <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="11" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5228,10 +5234,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4D1EB68-AD38-427D-9E4D-D27685135421}">
-  <dimension ref="A1:B30"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5374,6 +5380,14 @@
         <v>45593</v>
       </c>
     </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="427">
+        <v>45722</v>
+      </c>
+      <c r="B31" s="509" t="s">
+        <v>487</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5384,7 +5398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01683DA1-9EDF-4D0E-A820-BB1DCD1FA6A5}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A28" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -5401,7 +5415,7 @@
   <dimension ref="A1:AP140"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="G66" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="G133" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="A65" sqref="A65:XFD66"/>
@@ -23789,9 +23803,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79350F2F-5EA6-46A7-80B5-870BEBBCA740}">
   <dimension ref="A1:AR109"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25237,8 +25251,8 @@
       <c r="G17" s="454" t="s">
         <v>155</v>
       </c>
-      <c r="H17" s="447">
-        <v>1</v>
+      <c r="H17" s="561" t="s">
+        <v>155</v>
       </c>
       <c r="I17" s="156" t="str">
         <f>$E17</f>
@@ -33016,6 +33030,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -33096,7 +33111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9B1599C-D365-4B72-AD10-0C75C8355F18}">
   <dimension ref="A1:BO33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -39630,6 +39645,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010072E6CDABC94C8E4D9FF787BE52A12D70" ma:contentTypeVersion="12" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="d7db233095d5c438baabbd879a4c3a16">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b4710195-8c97-40d8-961f-382a10a2b3ee" xmlns:ns3="34f82a15-a147-4b49-8ecb-26ad79431260" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fcf6106967269ac970a9196950ae0a38" ns2:_="" ns3:_="">
     <xsd:import namespace="b4710195-8c97-40d8-961f-382a10a2b3ee"/>
@@ -39846,12 +39867,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1902ECF-A93E-435D-908F-0926C6EE1B5F}">
   <ds:schemaRefs>
@@ -39861,6 +39876,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E666C7DC-BABB-45EF-8C3F-0881662747CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b4710195-8c97-40d8-961f-382a10a2b3ee"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CBB2B996-2C85-4930-B3D3-5886FCC92095}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -39877,20 +39908,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E666C7DC-BABB-45EF-8C3F-0881662747CC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="b4710195-8c97-40d8-961f-382a10a2b3ee"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>